<commit_message>
Preedicting the impact of population on different aspects in Pakistan
</commit_message>
<xml_diff>
--- a/Refined/CleanData.xlsx
+++ b/Refined/CleanData.xlsx
@@ -1,81 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Ratio</t>
-  </si>
-  <si>
-    <t>Median Age</t>
-  </si>
-  <si>
-    <t>Increase Rate</t>
-  </si>
-  <si>
-    <t>Life Expectancy</t>
-  </si>
-  <si>
-    <t>Inflation</t>
-  </si>
-  <si>
-    <t>Unemployment</t>
-  </si>
-  <si>
-    <t>GDP</t>
-  </si>
-  <si>
-    <t>Homicides</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -90,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -406,2408 +420,2438 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Ratio</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Median Age</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Increase Rate</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Life Expectancy</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Inflation</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unemployment</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>GDP</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Homicides</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1960</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>45954.226</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>24795.178</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>21159.049</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>117.185</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>18.429</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>2.485</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>43.355</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="n">
         <v>6.94736842105289</v>
       </c>
-      <c r="J2">
-        <v>0.4</v>
-      </c>
-      <c r="K2">
+      <c r="J2" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K2" t="n">
         <v>3749265014.699707</v>
       </c>
-      <c r="L2">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3">
+      <c r="L2" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>1961</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>47060.915</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>25363.721</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>21697.194</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>116.899</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>18.36</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>2.277</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>44.18</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="n">
         <v>1.64041994750609</v>
       </c>
-      <c r="J3">
-        <v>0.4</v>
-      </c>
-      <c r="K3">
+      <c r="J3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K3" t="n">
         <v>4118647627.04746</v>
       </c>
-      <c r="L3">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4">
+      <c r="L3" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>1962</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>48161.841</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>25930.189</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>22231.652</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>116.636</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>18.271</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>2.347</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="n">
         <v>45.009</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="n">
         <v>-0.5164622336985</v>
       </c>
-      <c r="J4">
-        <v>0.4</v>
-      </c>
-      <c r="K4">
+      <c r="J4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K4" t="n">
         <v>4310163796.724066</v>
       </c>
-      <c r="L4">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5">
+      <c r="L4" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>1963</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>49325.05</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>26526.519</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>22798.53</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>116.352</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>18.183</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>2.425</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>46.318</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="n">
         <v>1.45648844797496</v>
       </c>
-      <c r="J5">
-        <v>0.4</v>
-      </c>
-      <c r="K5">
+      <c r="J5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K5" t="n">
         <v>4630827383.452332</v>
       </c>
-      <c r="L5">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6">
+      <c r="L5" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>1964</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>50552.592</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>27153.709</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>23398.883</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>116.047</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>18.084</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>2.49</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="n">
         <v>47.36</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="n">
         <v>4.17958688145319</v>
       </c>
-      <c r="J6">
-        <v>0.4</v>
-      </c>
-      <c r="K6">
+      <c r="J6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K6" t="n">
         <v>5204955900.881983</v>
       </c>
-      <c r="L6">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7">
+      <c r="L6" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>1965</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>51841.626</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>27810.773</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>24030.852</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>115.729</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>17.973</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="n">
         <v>2.545</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="n">
         <v>48.462</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="n">
         <v>5.56863547936375</v>
       </c>
-      <c r="J7">
-        <v>0.4</v>
-      </c>
-      <c r="K7">
+      <c r="J7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K7" t="n">
         <v>5929231415.371693</v>
       </c>
-      <c r="L7">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8">
+      <c r="L7" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>1966</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>53199.414</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>28501.4</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>24698.014</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>115.4</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="n">
         <v>17.852</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="n">
         <v>2.625</v>
       </c>
-      <c r="H8">
+      <c r="H8" t="n">
         <v>49.972</v>
       </c>
-      <c r="I8">
+      <c r="I8" t="n">
         <v>7.22762159787735</v>
       </c>
-      <c r="J8">
-        <v>0.4</v>
-      </c>
-      <c r="K8">
+      <c r="J8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K8" t="n">
         <v>6561108777.824444</v>
       </c>
-      <c r="L8">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9">
+      <c r="L8" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>1967</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>54629.793</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>29228.649</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>25401.143</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>115.068</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="n">
         <v>17.705</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n">
         <v>2.681</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="n">
         <v>51.16</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="n">
         <v>6.81139963428688</v>
       </c>
-      <c r="J9">
-        <v>0.4</v>
-      </c>
-      <c r="K9">
+      <c r="J9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K9" t="n">
         <v>7464510709.785805</v>
       </c>
-      <c r="L9">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10">
+      <c r="L9" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>1968</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>56124.743</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>29988.206</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>26136.537</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>114.737</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="n">
         <v>17.528</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="n">
         <v>2.718</v>
       </c>
-      <c r="H10">
+      <c r="H10" t="n">
         <v>52.281</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="n">
         <v>0.170627348438101</v>
       </c>
-      <c r="J10">
-        <v>0.4</v>
-      </c>
-      <c r="K10">
+      <c r="J10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K10" t="n">
         <v>8041999160.0168</v>
       </c>
-      <c r="L10">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11">
+      <c r="L10" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
         <v>1969</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>57676.805</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>30776.207</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>26900.599</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>114.407</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="n">
         <v>17.346</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="n">
         <v>2.737</v>
       </c>
-      <c r="H11">
+      <c r="H11" t="n">
         <v>53.276</v>
       </c>
-      <c r="I11">
+      <c r="I11" t="n">
         <v>3.18698679573686</v>
       </c>
-      <c r="J11">
-        <v>0.4</v>
-      </c>
-      <c r="K11">
+      <c r="J11" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K11" t="n">
         <v>8683116337.673246</v>
       </c>
-      <c r="L11">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12">
+      <c r="L11" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>1970</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>59290.872</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>31594.424</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>27696.448</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>114.074</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="n">
         <v>17.199</v>
       </c>
-      <c r="G12">
+      <c r="G12" t="n">
         <v>2.782</v>
       </c>
-      <c r="H12">
+      <c r="H12" t="n">
         <v>54.57</v>
       </c>
-      <c r="I12">
+      <c r="I12" t="n">
         <v>5.34984090983017</v>
       </c>
-      <c r="J12">
-        <v>0.4</v>
-      </c>
-      <c r="K12">
+      <c r="J12" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K12" t="n">
         <v>10027509449.811</v>
       </c>
-      <c r="L12">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13">
+      <c r="L12" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
         <v>1971</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>60878.781</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="n">
         <v>32382.253</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="n">
         <v>28496.527</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>113.636</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="n">
         <v>17.074</v>
       </c>
-      <c r="G13">
+      <c r="G13" t="n">
         <v>2.507</v>
       </c>
-      <c r="H13">
+      <c r="H13" t="n">
         <v>52.15</v>
       </c>
-      <c r="I13">
+      <c r="I13" t="n">
         <v>4.73069148232272</v>
       </c>
-      <c r="J13">
-        <v>0.4</v>
-      </c>
-      <c r="K13">
+      <c r="J13" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K13" t="n">
         <v>10665896682.06636</v>
       </c>
-      <c r="L13">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14">
+      <c r="L13" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>1972</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>62509.565</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>33192.037</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>29317.529</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>113.216</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="n">
         <v>16.972</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="n">
         <v>2.776</v>
       </c>
-      <c r="H14">
+      <c r="H14" t="n">
         <v>55.146</v>
       </c>
-      <c r="I14">
+      <c r="I14" t="n">
         <v>5.18323764549138</v>
       </c>
-      <c r="J14">
-        <v>0.4</v>
-      </c>
-      <c r="K14">
+      <c r="J14" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K14" t="n">
         <v>9415016359.56604</v>
       </c>
-      <c r="L14">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15">
+      <c r="L14" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
         <v>1973</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>64285.624</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>34091.252</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="n">
         <v>30194.373</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>112.906</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="n">
         <v>16.902</v>
       </c>
-      <c r="G15">
+      <c r="G15" t="n">
         <v>2.826</v>
       </c>
-      <c r="H15">
+      <c r="H15" t="n">
         <v>55.546</v>
       </c>
-      <c r="I15">
+      <c r="I15" t="n">
         <v>23.0700840250844</v>
       </c>
-      <c r="J15">
-        <v>0.4</v>
-      </c>
-      <c r="K15">
+      <c r="J15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K15" t="n">
         <v>6383429490.210915</v>
       </c>
-      <c r="L15">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16">
+      <c r="L15" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
         <v>1974</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>66149.16899999999</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>35033.843</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>31115.326</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>112.594</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="n">
         <v>16.86</v>
       </c>
-      <c r="G16">
+      <c r="G16" t="n">
         <v>2.888</v>
       </c>
-      <c r="H16">
+      <c r="H16" t="n">
         <v>55.607</v>
       </c>
-      <c r="I16">
+      <c r="I16" t="n">
         <v>26.6630348537488</v>
       </c>
-      <c r="J16">
-        <v>0.4</v>
-      </c>
-      <c r="K16">
+      <c r="J16" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K16" t="n">
         <v>8899191919.191919</v>
       </c>
-      <c r="L16">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17">
+      <c r="L16" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
         <v>1975</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>68126.999</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="n">
         <v>36033.414</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="n">
         <v>32093.585</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="n">
         <v>112.276</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="n">
         <v>16.849</v>
       </c>
-      <c r="G17">
+      <c r="G17" t="n">
         <v>3.003</v>
       </c>
-      <c r="H17">
+      <c r="H17" t="n">
         <v>56.175</v>
       </c>
-      <c r="I17">
+      <c r="I17" t="n">
         <v>20.9045094573998</v>
       </c>
-      <c r="J17">
-        <v>0.4</v>
-      </c>
-      <c r="K17">
+      <c r="J17" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K17" t="n">
         <v>11230606060.60606</v>
       </c>
-      <c r="L17">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18">
+      <c r="L17" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
         <v>1976</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>70230.923</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>37095.743</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="n">
         <v>33135.18</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>111.953</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="n">
         <v>16.865</v>
       </c>
-      <c r="G18">
+      <c r="G18" t="n">
         <v>3.079</v>
       </c>
-      <c r="H18">
+      <c r="H18" t="n">
         <v>56.517</v>
       </c>
-      <c r="I18">
+      <c r="I18" t="n">
         <v>7.15832373118465</v>
       </c>
-      <c r="J18">
-        <v>0.4</v>
-      </c>
-      <c r="K18">
+      <c r="J18" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K18" t="n">
         <v>13168080808.08081</v>
       </c>
-      <c r="L18">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19">
+      <c r="L18" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
         <v>1977</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="n">
         <v>72451.105</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="n">
         <v>38216.474</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="n">
         <v>34234.632</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>111.631</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="n">
         <v>16.899</v>
       </c>
-      <c r="G19">
+      <c r="G19" t="n">
         <v>3.144</v>
       </c>
-      <c r="H19">
+      <c r="H19" t="n">
         <v>56.857</v>
       </c>
-      <c r="I19">
+      <c r="I19" t="n">
         <v>10.1329676874055</v>
       </c>
-      <c r="J19">
-        <v>0.4</v>
-      </c>
-      <c r="K19">
+      <c r="J19" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K19" t="n">
         <v>15126060606.06061</v>
       </c>
-      <c r="L19">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20">
+      <c r="L19" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
         <v>1978</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>74789.33</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="n">
         <v>39396.326</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="n">
         <v>35393.003</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="n">
         <v>111.311</v>
       </c>
-      <c r="F20">
+      <c r="F20" t="n">
         <v>16.943</v>
       </c>
-      <c r="G20">
+      <c r="G20" t="n">
         <v>3.207</v>
       </c>
-      <c r="H20">
+      <c r="H20" t="n">
         <v>57.398</v>
       </c>
-      <c r="I20">
+      <c r="I20" t="n">
         <v>6.13869266742743</v>
       </c>
-      <c r="J20">
-        <v>0.4</v>
-      </c>
-      <c r="K20">
+      <c r="J20" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K20" t="n">
         <v>17811515151.51515</v>
       </c>
-      <c r="L20">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21">
+      <c r="L20" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
         <v>1979</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>77407.341</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="n">
         <v>40711.907</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="n">
         <v>36695.434</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="n">
         <v>110.945</v>
       </c>
-      <c r="F21">
+      <c r="F21" t="n">
         <v>17.028</v>
       </c>
-      <c r="G21">
+      <c r="G21" t="n">
         <v>3.666</v>
       </c>
-      <c r="H21">
+      <c r="H21" t="n">
         <v>58.084</v>
       </c>
-      <c r="I21">
+      <c r="I21" t="n">
         <v>8.26704697617572</v>
       </c>
-      <c r="J21">
-        <v>0.4</v>
-      </c>
-      <c r="K21">
+      <c r="J21" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K21" t="n">
         <v>19688383838.38384</v>
       </c>
-      <c r="L21">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22">
+      <c r="L21" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
         <v>1980</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>80624.057</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="n">
         <v>42323.346</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="n">
         <v>38300.711</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="n">
         <v>110.503</v>
       </c>
-      <c r="F22">
+      <c r="F22" t="n">
         <v>17.203</v>
       </c>
-      <c r="G22">
+      <c r="G22" t="n">
         <v>4.461</v>
       </c>
-      <c r="H22">
+      <c r="H22" t="n">
         <v>58.642</v>
       </c>
-      <c r="I22">
+      <c r="I22" t="n">
         <v>11.9382309107087</v>
       </c>
-      <c r="J22">
-        <v>0.4</v>
-      </c>
-      <c r="K22">
+      <c r="J22" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K22" t="n">
         <v>23654444444.44444</v>
       </c>
-      <c r="L22">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23">
+      <c r="L22" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
         <v>1981</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="n">
         <v>84270.202</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="n">
         <v>44149.23</v>
       </c>
-      <c r="D23">
+      <c r="D23" t="n">
         <v>40120.973</v>
       </c>
-      <c r="E23">
+      <c r="E23" t="n">
         <v>110.04</v>
       </c>
-      <c r="F23">
+      <c r="F23" t="n">
         <v>17.406</v>
       </c>
-      <c r="G23">
+      <c r="G23" t="n">
         <v>4.387</v>
       </c>
-      <c r="H23">
+      <c r="H23" t="n">
         <v>59.301</v>
       </c>
-      <c r="I23">
+      <c r="I23" t="n">
         <v>11.8799135925283</v>
       </c>
-      <c r="J23">
-        <v>0.4</v>
-      </c>
-      <c r="K23">
+      <c r="J23" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K23" t="n">
         <v>28100606060.60606</v>
       </c>
-      <c r="L23">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24">
+      <c r="L23" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
         <v>1982</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="n">
         <v>87828.198</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="n">
         <v>45930.13</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="n">
         <v>41898.068</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="n">
         <v>109.624</v>
       </c>
-      <c r="F24">
+      <c r="F24" t="n">
         <v>17.532</v>
       </c>
-      <c r="G24">
+      <c r="G24" t="n">
         <v>3.894</v>
       </c>
-      <c r="H24">
+      <c r="H24" t="n">
         <v>59.802</v>
       </c>
-      <c r="I24">
+      <c r="I24" t="n">
         <v>5.90352878435863</v>
       </c>
-      <c r="J24">
-        <v>0.4</v>
-      </c>
-      <c r="K24">
+      <c r="J24" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K24" t="n">
         <v>30725971563.98104</v>
       </c>
-      <c r="L24">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25">
+      <c r="L24" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
         <v>1983</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="n">
         <v>91080.372</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="n">
         <v>47557.446</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="n">
         <v>43522.925</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="n">
         <v>109.27</v>
       </c>
-      <c r="F25">
+      <c r="F25" t="n">
         <v>17.555</v>
       </c>
-      <c r="G25">
+      <c r="G25" t="n">
         <v>3.387</v>
       </c>
-      <c r="H25">
+      <c r="H25" t="n">
         <v>60.499</v>
       </c>
-      <c r="I25">
+      <c r="I25" t="n">
         <v>6.362033499853</v>
       </c>
-      <c r="J25">
-        <v>0.4</v>
-      </c>
-      <c r="K25">
+      <c r="J25" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K25" t="n">
         <v>28691889763.77953</v>
       </c>
-      <c r="L25">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26">
+      <c r="L25" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
         <v>1984</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="n">
         <v>94003.867</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="n">
         <v>49019.878</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="n">
         <v>44983.988</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>108.972</v>
       </c>
-      <c r="F26">
+      <c r="F26" t="n">
         <v>17.487</v>
       </c>
-      <c r="G26">
+      <c r="G26" t="n">
         <v>2.939</v>
       </c>
-      <c r="H26">
+      <c r="H26" t="n">
         <v>61.01</v>
       </c>
-      <c r="I26">
+      <c r="I26" t="n">
         <v>6.08716673573716</v>
       </c>
-      <c r="J26">
-        <v>0.4</v>
-      </c>
-      <c r="K26">
+      <c r="J26" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K26" t="n">
         <v>31151825467.49777</v>
       </c>
-      <c r="L26">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27">
+      <c r="L26" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
         <v>1985</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="n">
         <v>97121.552</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="n">
         <v>50585.068</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="n">
         <v>46536.484</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>108.7</v>
       </c>
-      <c r="F27">
+      <c r="F27" t="n">
         <v>17.429</v>
       </c>
-      <c r="G27">
+      <c r="G27" t="n">
         <v>3.576</v>
       </c>
-      <c r="H27">
+      <c r="H27" t="n">
         <v>60.403</v>
       </c>
-      <c r="I27">
+      <c r="I27" t="n">
         <v>5.61483921793224</v>
       </c>
-      <c r="J27">
-        <v>0.4</v>
-      </c>
-      <c r="K27">
+      <c r="J27" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K27" t="n">
         <v>31144920844.32718</v>
       </c>
-      <c r="L27">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28">
+      <c r="L27" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
         <v>1986</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="n">
         <v>100618.523</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="n">
         <v>52349.211</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="n">
         <v>48269.312</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="n">
         <v>108.452</v>
       </c>
-      <c r="F28">
+      <c r="F28" t="n">
         <v>17.403</v>
       </c>
-      <c r="G28">
+      <c r="G28" t="n">
         <v>3.5</v>
       </c>
-      <c r="H28">
+      <c r="H28" t="n">
         <v>60.252</v>
       </c>
-      <c r="I28">
+      <c r="I28" t="n">
         <v>3.50641424758205</v>
       </c>
-      <c r="J28">
-        <v>0.4</v>
-      </c>
-      <c r="K28">
+      <c r="J28" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K28" t="n">
         <v>31899070055.79665</v>
       </c>
-      <c r="L28">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29">
+      <c r="L28" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
         <v>1987</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="n">
         <v>104251.093</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="n">
         <v>54186.251</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="n">
         <v>50064.842</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="n">
         <v>108.232</v>
       </c>
-      <c r="F29">
+      <c r="F29" t="n">
         <v>17.361</v>
       </c>
-      <c r="G29">
+      <c r="G29" t="n">
         <v>3.592</v>
       </c>
-      <c r="H29">
+      <c r="H29" t="n">
         <v>59.782</v>
       </c>
-      <c r="I29">
+      <c r="I29" t="n">
         <v>4.68121854620213</v>
       </c>
-      <c r="J29">
-        <v>0.4</v>
-      </c>
-      <c r="K29">
+      <c r="J29" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K29" t="n">
         <v>33351529274.68686</v>
       </c>
-      <c r="L29">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30">
+      <c r="L29" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
         <v>1988</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="n">
         <v>107967.838</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="n">
         <v>56068.126</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="n">
         <v>51899.712</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="n">
         <v>108.032</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="n">
         <v>17.301</v>
       </c>
-      <c r="G30">
+      <c r="G30" t="n">
         <v>3.417</v>
       </c>
-      <c r="H30">
+      <c r="H30" t="n">
         <v>60.377</v>
       </c>
-      <c r="I30">
+      <c r="I30" t="n">
         <v>8.83793701817773</v>
       </c>
-      <c r="J30">
-        <v>0.4</v>
-      </c>
-      <c r="K30">
+      <c r="J30" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K30" t="n">
         <v>38472742808.31672</v>
       </c>
-      <c r="L30">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31">
+      <c r="L30" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
         <v>1989</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="n">
         <v>111670.386</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="n">
         <v>57945.452</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="n">
         <v>53724.935</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>107.856</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="n">
         <v>17.217</v>
       </c>
-      <c r="G31">
+      <c r="G31" t="n">
         <v>3.328</v>
       </c>
-      <c r="H31">
+      <c r="H31" t="n">
         <v>60.731</v>
       </c>
-      <c r="I31">
+      <c r="I31" t="n">
         <v>7.84426473740044</v>
       </c>
-      <c r="J31">
-        <v>0.4</v>
-      </c>
-      <c r="K31">
+      <c r="J31" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K31" t="n">
         <v>40171106279.0078</v>
       </c>
-      <c r="L31">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32">
+      <c r="L31" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
         <v>1990</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="n">
         <v>115414.069</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="n">
         <v>59844.215</v>
       </c>
-      <c r="D32">
+      <c r="D32" t="n">
         <v>55569.854</v>
       </c>
-      <c r="E32">
+      <c r="E32" t="n">
         <v>107.692</v>
       </c>
-      <c r="F32">
+      <c r="F32" t="n">
         <v>17.132</v>
       </c>
-      <c r="G32">
+      <c r="G32" t="n">
         <v>3.268</v>
       </c>
-      <c r="H32">
+      <c r="H32" t="n">
         <v>61.409</v>
       </c>
-      <c r="I32">
+      <c r="I32" t="n">
         <v>9.052131552797761</v>
       </c>
-      <c r="J32">
-        <v>0.4</v>
-      </c>
-      <c r="K32">
+      <c r="J32" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K32" t="n">
         <v>40010423970.45763</v>
       </c>
-      <c r="L32">
+      <c r="L32" t="n">
         <v>7.11265102735157</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
-      <c r="A33">
+    <row r="33">
+      <c r="A33" t="n">
         <v>1991</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="n">
         <v>119203.569</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="n">
         <v>61767.894</v>
       </c>
-      <c r="D33">
+      <c r="D33" t="n">
         <v>57435.675</v>
       </c>
-      <c r="E33">
+      <c r="E33" t="n">
         <v>107.543</v>
       </c>
-      <c r="F33">
+      <c r="F33" t="n">
         <v>17.054</v>
       </c>
-      <c r="G33">
+      <c r="G33" t="n">
         <v>3.194</v>
       </c>
-      <c r="H33">
+      <c r="H33" t="n">
         <v>61.331</v>
       </c>
-      <c r="I33">
+      <c r="I33" t="n">
         <v>11.7912703351416</v>
       </c>
-      <c r="J33">
+      <c r="J33" t="n">
         <v>0.583</v>
       </c>
-      <c r="K33">
+      <c r="K33" t="n">
         <v>45625336680.20465</v>
       </c>
-      <c r="L33">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34">
+      <c r="L33" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
         <v>1992</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="n">
         <v>122375.179</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="n">
         <v>63389.141</v>
       </c>
-      <c r="D34">
+      <c r="D34" t="n">
         <v>58986.038</v>
       </c>
-      <c r="E34">
+      <c r="E34" t="n">
         <v>107.465</v>
       </c>
-      <c r="F34">
+      <c r="F34" t="n">
         <v>16.89</v>
       </c>
-      <c r="G34">
+      <c r="G34" t="n">
         <v>2.072</v>
       </c>
-      <c r="H34">
+      <c r="H34" t="n">
         <v>60.733</v>
       </c>
-      <c r="I34">
+      <c r="I34" t="n">
         <v>9.5090414619015</v>
       </c>
-      <c r="J34">
+      <c r="J34" t="n">
         <v>0.583</v>
       </c>
-      <c r="K34">
+      <c r="K34" t="n">
         <v>48884671947.46571</v>
       </c>
-      <c r="L34">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35">
+      <c r="L34" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
         <v>1993</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="n">
         <v>125546.615</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="n">
         <v>65019.628</v>
       </c>
-      <c r="D35">
+      <c r="D35" t="n">
         <v>60526.987</v>
       </c>
-      <c r="E35">
+      <c r="E35" t="n">
         <v>107.423</v>
       </c>
-      <c r="F35">
+      <c r="F35" t="n">
         <v>16.746</v>
       </c>
-      <c r="G35">
+      <c r="G35" t="n">
         <v>3.033</v>
       </c>
-      <c r="H35">
+      <c r="H35" t="n">
         <v>60.369</v>
       </c>
-      <c r="I35">
+      <c r="I35" t="n">
         <v>9.97366476029209</v>
       </c>
-      <c r="J35">
+      <c r="J35" t="n">
         <v>0.585</v>
       </c>
-      <c r="K35">
+      <c r="K35" t="n">
         <v>51809999353.16135</v>
       </c>
-      <c r="L35">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36">
+      <c r="L35" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
         <v>1994</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="n">
         <v>129245.139</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="n">
         <v>66919.87699999999</v>
       </c>
-      <c r="D36">
+      <c r="D36" t="n">
         <v>62325.262</v>
       </c>
-      <c r="E36">
+      <c r="E36" t="n">
         <v>107.372</v>
       </c>
-      <c r="F36">
+      <c r="F36" t="n">
         <v>16.7</v>
       </c>
-      <c r="G36">
+      <c r="G36" t="n">
         <v>2.778</v>
       </c>
-      <c r="H36">
+      <c r="H36" t="n">
         <v>60.634</v>
       </c>
-      <c r="I36">
+      <c r="I36" t="n">
         <v>12.3681943936948</v>
       </c>
-      <c r="J36">
+      <c r="J36" t="n">
         <v>0.585</v>
       </c>
-      <c r="K36">
+      <c r="K36" t="n">
         <v>52293470813.13361</v>
       </c>
-      <c r="L36">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37">
+      <c r="L36" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
         <v>1995</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="n">
         <v>133117.476</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="n">
         <v>68906.276</v>
       </c>
-      <c r="D37">
+      <c r="D37" t="n">
         <v>64211.2</v>
       </c>
-      <c r="E37">
+      <c r="E37" t="n">
         <v>107.312</v>
       </c>
-      <c r="F37">
+      <c r="F37" t="n">
         <v>16.696</v>
       </c>
-      <c r="G37">
+      <c r="G37" t="n">
         <v>3.121</v>
       </c>
-      <c r="H37">
+      <c r="H37" t="n">
         <v>60.391</v>
       </c>
-      <c r="I37">
+      <c r="I37" t="n">
         <v>12.3435785170513</v>
       </c>
-      <c r="J37">
+      <c r="J37" t="n">
         <v>0.586</v>
       </c>
-      <c r="K37">
+      <c r="K37" t="n">
         <v>60636071684.1918</v>
       </c>
-      <c r="L37">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
-      <c r="A38">
+      <c r="L37" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
         <v>1996</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="n">
         <v>137234.81</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="n">
         <v>71012.95299999999</v>
       </c>
-      <c r="D38">
+      <c r="D38" t="n">
         <v>66221.856</v>
       </c>
-      <c r="E38">
+      <c r="E38" t="n">
         <v>107.235</v>
       </c>
-      <c r="F38">
+      <c r="F38" t="n">
         <v>16.742</v>
       </c>
-      <c r="G38">
+      <c r="G38" t="n">
         <v>2.973</v>
       </c>
-      <c r="H38">
+      <c r="H38" t="n">
         <v>61.062</v>
       </c>
-      <c r="I38">
+      <c r="I38" t="n">
         <v>10.3738085885002</v>
       </c>
-      <c r="J38">
+      <c r="J38" t="n">
         <v>0.585</v>
       </c>
-      <c r="K38">
+      <c r="K38" t="n">
         <v>63320170084.40755</v>
       </c>
-      <c r="L38">
+      <c r="L38" t="n">
         <v>6.60328092633087</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
-      <c r="A39">
+    <row r="39">
+      <c r="A39" t="n">
         <v>1997</v>
       </c>
-      <c r="B39">
+      <c r="B39" t="n">
         <v>141330.267</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="n">
         <v>73104.663</v>
       </c>
-      <c r="D39">
+      <c r="D39" t="n">
         <v>68225.605</v>
       </c>
-      <c r="E39">
+      <c r="E39" t="n">
         <v>107.151</v>
       </c>
-      <c r="F39">
+      <c r="F39" t="n">
         <v>16.802</v>
       </c>
-      <c r="G39">
+      <c r="G39" t="n">
         <v>2.909</v>
       </c>
-      <c r="H39">
+      <c r="H39" t="n">
         <v>61.486</v>
       </c>
-      <c r="I39">
+      <c r="I39" t="n">
         <v>11.3754928865122</v>
       </c>
-      <c r="J39">
+      <c r="J39" t="n">
         <v>0.586</v>
       </c>
-      <c r="K39">
+      <c r="K39" t="n">
         <v>62433340468.02277</v>
       </c>
-      <c r="L39">
+      <c r="L39" t="n">
         <v>6.58316167129592</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
-      <c r="A40">
+    <row r="40">
+      <c r="A40" t="n">
         <v>1998</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="n">
         <v>145476.106</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="n">
         <v>75217.269</v>
       </c>
-      <c r="D40">
+      <c r="D40" t="n">
         <v>70258.836</v>
       </c>
-      <c r="E40">
+      <c r="E40" t="n">
         <v>107.057</v>
       </c>
-      <c r="F40">
+      <c r="F40" t="n">
         <v>16.886</v>
       </c>
-      <c r="G40">
+      <c r="G40" t="n">
         <v>2.874</v>
       </c>
-      <c r="H40">
+      <c r="H40" t="n">
         <v>62.112</v>
       </c>
-      <c r="I40">
+      <c r="I40" t="n">
         <v>6.22800415424543</v>
       </c>
-      <c r="J40">
+      <c r="J40" t="n">
         <v>0.587</v>
       </c>
-      <c r="K40">
+      <c r="K40" t="n">
         <v>62191955814.3478</v>
       </c>
-      <c r="L40">
+      <c r="L40" t="n">
         <v>7.04308103711231</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
-      <c r="A41">
+    <row r="41">
+      <c r="A41" t="n">
         <v>1999</v>
       </c>
-      <c r="B41">
+      <c r="B41" t="n">
         <v>149694.462</v>
       </c>
-      <c r="C41">
+      <c r="C41" t="n">
         <v>77366.201</v>
       </c>
-      <c r="D41">
+      <c r="D41" t="n">
         <v>72328.261</v>
       </c>
-      <c r="E41">
+      <c r="E41" t="n">
         <v>106.965</v>
       </c>
-      <c r="F41">
+      <c r="F41" t="n">
         <v>16.998</v>
       </c>
-      <c r="G41">
+      <c r="G41" t="n">
         <v>2.843</v>
       </c>
-      <c r="H41">
+      <c r="H41" t="n">
         <v>62.755</v>
       </c>
-      <c r="I41">
+      <c r="I41" t="n">
         <v>4.14263718082171</v>
       </c>
-      <c r="J41">
+      <c r="J41" t="n">
         <v>0.587</v>
       </c>
-      <c r="K41">
+      <c r="K41" t="n">
         <v>62973857068.51128</v>
       </c>
-      <c r="L41">
+      <c r="L41" t="n">
         <v>6.2340315568922</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
-      <c r="A42">
+    <row r="42">
+      <c r="A42" t="n">
         <v>2000</v>
       </c>
-      <c r="B42">
+      <c r="B42" t="n">
         <v>154369.924</v>
       </c>
-      <c r="C42">
+      <c r="C42" t="n">
         <v>79746.052</v>
       </c>
-      <c r="D42">
+      <c r="D42" t="n">
         <v>74623.871</v>
       </c>
-      <c r="E42">
+      <c r="E42" t="n">
         <v>106.864</v>
       </c>
-      <c r="F42">
+      <c r="F42" t="n">
         <v>17.18</v>
       </c>
-      <c r="G42">
+      <c r="G42" t="n">
         <v>3.301</v>
       </c>
-      <c r="H42">
+      <c r="H42" t="n">
         <v>63.124</v>
       </c>
-      <c r="I42">
+      <c r="I42" t="n">
         <v>4.36666451291681</v>
       </c>
-      <c r="J42">
+      <c r="J42" t="n">
         <v>0.585</v>
       </c>
-      <c r="K42">
+      <c r="K42" t="n">
         <v>99484802344.52766</v>
       </c>
-      <c r="L42">
+      <c r="L42" t="n">
         <v>5.76925854342345</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
-      <c r="A43">
+    <row r="43">
+      <c r="A43" t="n">
         <v>2001</v>
       </c>
-      <c r="B43">
+      <c r="B43" t="n">
         <v>159217.727</v>
       </c>
-      <c r="C43">
+      <c r="C43" t="n">
         <v>82212.66800000001</v>
       </c>
-      <c r="D43">
+      <c r="D43" t="n">
         <v>77005.05899999999</v>
       </c>
-      <c r="E43">
+      <c r="E43" t="n">
         <v>106.763</v>
       </c>
-      <c r="F43">
+      <c r="F43" t="n">
         <v>17.388</v>
       </c>
-      <c r="G43">
+      <c r="G43" t="n">
         <v>2.89</v>
       </c>
-      <c r="H43">
+      <c r="H43" t="n">
         <v>63.575</v>
       </c>
-      <c r="I43">
+      <c r="I43" t="n">
         <v>3.14826144590618</v>
       </c>
-      <c r="J43">
+      <c r="J43" t="n">
         <v>0.585</v>
       </c>
-      <c r="K43">
+      <c r="K43" t="n">
         <v>97145618479.90381</v>
       </c>
-      <c r="L43">
+      <c r="L43" t="n">
         <v>6.02508287283865</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
-      <c r="A44">
+    <row r="44">
+      <c r="A44" t="n">
         <v>2002</v>
       </c>
-      <c r="B44">
+      <c r="B44" t="n">
         <v>163262.807</v>
       </c>
-      <c r="C44">
+      <c r="C44" t="n">
         <v>84278.393</v>
       </c>
-      <c r="D44">
+      <c r="D44" t="n">
         <v>78984.41499999999</v>
       </c>
-      <c r="E44">
+      <c r="E44" t="n">
         <v>106.703</v>
       </c>
-      <c r="F44">
+      <c r="F44" t="n">
         <v>17.521</v>
       </c>
-      <c r="G44">
+      <c r="G44" t="n">
         <v>2.137</v>
       </c>
-      <c r="H44">
+      <c r="H44" t="n">
         <v>63.65</v>
       </c>
-      <c r="I44">
+      <c r="I44" t="n">
         <v>3.29034472613153</v>
       </c>
-      <c r="J44">
+      <c r="J44" t="n">
         <v>0.585</v>
       </c>
-      <c r="K44">
+      <c r="K44" t="n">
         <v>97923302809.35368</v>
       </c>
-      <c r="L44">
+      <c r="L44" t="n">
         <v>5.79801373316455</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
-      <c r="A45">
+    <row r="45">
+      <c r="A45" t="n">
         <v>2003</v>
       </c>
-      <c r="B45">
+      <c r="B45" t="n">
         <v>166876.68</v>
       </c>
-      <c r="C45">
+      <c r="C45" t="n">
         <v>86127.265</v>
       </c>
-      <c r="D45">
+      <c r="D45" t="n">
         <v>80749.416</v>
       </c>
-      <c r="E45">
+      <c r="E45" t="n">
         <v>106.66</v>
       </c>
-      <c r="F45">
+      <c r="F45" t="n">
         <v>17.623</v>
       </c>
-      <c r="G45">
+      <c r="G45" t="n">
         <v>2.24</v>
       </c>
-      <c r="H45">
+      <c r="H45" t="n">
         <v>63.967</v>
       </c>
-      <c r="I45">
+      <c r="I45" t="n">
         <v>2.91413470059479</v>
       </c>
-      <c r="J45">
+      <c r="J45" t="n">
         <v>0.584</v>
       </c>
-      <c r="K45">
+      <c r="K45" t="n">
         <v>112371913740.823</v>
       </c>
-      <c r="L45">
+      <c r="L45" t="n">
         <v>5.60054285116248</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
-      <c r="A46">
+    <row r="46">
+      <c r="A46" t="n">
         <v>2004</v>
       </c>
-      <c r="B46">
+      <c r="B46" t="n">
         <v>170648.62</v>
       </c>
-      <c r="C46">
+      <c r="C46" t="n">
         <v>88049.526</v>
       </c>
-      <c r="D46">
+      <c r="D46" t="n">
         <v>82599.094</v>
       </c>
-      <c r="E46">
+      <c r="E46" t="n">
         <v>106.599</v>
       </c>
-      <c r="F46">
+      <c r="F46" t="n">
         <v>17.754</v>
       </c>
-      <c r="G46">
+      <c r="G46" t="n">
         <v>2.23</v>
       </c>
-      <c r="H46">
+      <c r="H46" t="n">
         <v>64.40900000000001</v>
       </c>
-      <c r="I46">
+      <c r="I46" t="n">
         <v>7.44462469342739</v>
       </c>
-      <c r="J46">
+      <c r="J46" t="n">
         <v>0.582</v>
       </c>
-      <c r="K46">
+      <c r="K46" t="n">
         <v>132216048339.4129</v>
       </c>
-      <c r="L46">
+      <c r="L46" t="n">
         <v>5.63379885521489</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
-      <c r="A47">
+    <row r="47">
+      <c r="A47" t="n">
         <v>2005</v>
       </c>
-      <c r="B47">
+      <c r="B47" t="n">
         <v>174372.098</v>
       </c>
-      <c r="C47">
+      <c r="C47" t="n">
         <v>89942.008</v>
       </c>
-      <c r="D47">
+      <c r="D47" t="n">
         <v>84430.09</v>
       </c>
-      <c r="E47">
+      <c r="E47" t="n">
         <v>106.528</v>
       </c>
-      <c r="F47">
+      <c r="F47" t="n">
         <v>17.9</v>
       </c>
-      <c r="G47">
+      <c r="G47" t="n">
         <v>2.088</v>
       </c>
-      <c r="H47">
+      <c r="H47" t="n">
         <v>63.967</v>
       </c>
-      <c r="I47">
+      <c r="I47" t="n">
         <v>9.063327370304171</v>
       </c>
-      <c r="J47">
+      <c r="J47" t="n">
         <v>0.58</v>
       </c>
-      <c r="K47">
+      <c r="K47" t="n">
         <v>145208562960.7666</v>
       </c>
-      <c r="L47">
+      <c r="L47" t="n">
         <v>5.60984246458972</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
-      <c r="A48">
+    <row r="48">
+      <c r="A48" t="n">
         <v>2006</v>
       </c>
-      <c r="B48">
+      <c r="B48" t="n">
         <v>178069.984</v>
       </c>
-      <c r="C48">
+      <c r="C48" t="n">
         <v>91810.143</v>
       </c>
-      <c r="D48">
+      <c r="D48" t="n">
         <v>86259.841</v>
       </c>
-      <c r="E48">
+      <c r="E48" t="n">
         <v>106.434</v>
       </c>
-      <c r="F48">
+      <c r="F48" t="n">
         <v>18.061</v>
       </c>
-      <c r="G48">
+      <c r="G48" t="n">
         <v>2.108</v>
       </c>
-      <c r="H48">
+      <c r="H48" t="n">
         <v>65.65300000000001</v>
       </c>
-      <c r="I48">
+      <c r="I48" t="n">
         <v>7.92108440058789</v>
       </c>
-      <c r="J48">
+      <c r="J48" t="n">
         <v>0.58</v>
       </c>
-      <c r="K48">
+      <c r="K48" t="n">
         <v>161871385506.3602</v>
       </c>
-      <c r="L48">
+      <c r="L48" t="n">
         <v>5.64272526232516</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
-      <c r="A49">
+    <row r="49">
+      <c r="A49" t="n">
         <v>2007</v>
       </c>
-      <c r="B49">
+      <c r="B49" t="n">
         <v>181924.521</v>
       </c>
-      <c r="C49">
+      <c r="C49" t="n">
         <v>93744.001</v>
       </c>
-      <c r="D49">
+      <c r="D49" t="n">
         <v>88180.519</v>
       </c>
-      <c r="E49">
+      <c r="E49" t="n">
         <v>106.309</v>
       </c>
-      <c r="F49">
+      <c r="F49" t="n">
         <v>18.231</v>
       </c>
-      <c r="G49">
+      <c r="G49" t="n">
         <v>2.174</v>
       </c>
-      <c r="H49">
+      <c r="H49" t="n">
         <v>66.10299999999999</v>
       </c>
-      <c r="I49">
+      <c r="I49" t="n">
         <v>7.59868441050774</v>
       </c>
-      <c r="J49">
-        <v>0.4</v>
-      </c>
-      <c r="K49">
+      <c r="J49" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K49" t="n">
         <v>184140869997.4602</v>
       </c>
-      <c r="L49">
+      <c r="L49" t="n">
         <v>5.80240638864292</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
-      <c r="A50">
+    <row r="50">
+      <c r="A50" t="n">
         <v>2008</v>
       </c>
-      <c r="B50">
+      <c r="B50" t="n">
         <v>185931.955</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="n">
         <v>95745.628</v>
       </c>
-      <c r="D50">
+      <c r="D50" t="n">
         <v>90186.327</v>
       </c>
-      <c r="E50">
+      <c r="E50" t="n">
         <v>106.164</v>
       </c>
-      <c r="F50">
+      <c r="F50" t="n">
         <v>18.408</v>
       </c>
-      <c r="G50">
+      <c r="G50" t="n">
         <v>2.184</v>
       </c>
-      <c r="H50">
+      <c r="H50" t="n">
         <v>66.5</v>
       </c>
-      <c r="I50">
+      <c r="I50" t="n">
         <v>20.2861210929554</v>
       </c>
-      <c r="J50">
+      <c r="J50" t="n">
         <v>0.42</v>
       </c>
-      <c r="K50">
+      <c r="K50" t="n">
         <v>202203748583.8536</v>
       </c>
-      <c r="L50">
+      <c r="L50" t="n">
         <v>6.48570602078594</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
-      <c r="A51">
+    <row r="51">
+      <c r="A51" t="n">
         <v>2009</v>
       </c>
-      <c r="B51">
+      <c r="B51" t="n">
         <v>190123.222</v>
       </c>
-      <c r="C51">
+      <c r="C51" t="n">
         <v>97833.204</v>
       </c>
-      <c r="D51">
+      <c r="D51" t="n">
         <v>92290.019</v>
       </c>
-      <c r="E51">
+      <c r="E51" t="n">
         <v>106.006</v>
       </c>
-      <c r="F51">
+      <c r="F51" t="n">
         <v>18.596</v>
       </c>
-      <c r="G51">
+      <c r="G51" t="n">
         <v>2.274</v>
       </c>
-      <c r="H51">
+      <c r="H51" t="n">
         <v>66.53100000000001</v>
       </c>
-      <c r="I51">
+      <c r="I51" t="n">
         <v>13.6477650639761</v>
       </c>
-      <c r="J51">
+      <c r="J51" t="n">
         <v>0.54</v>
       </c>
-      <c r="K51">
+      <c r="K51" t="n">
         <v>187337783856.4657</v>
       </c>
-      <c r="L51">
+      <c r="L51" t="n">
         <v>6.56994967190278</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
-      <c r="A52">
+    <row r="52">
+      <c r="A52" t="n">
         <v>2010</v>
       </c>
-      <c r="B52">
+      <c r="B52" t="n">
         <v>194454.498</v>
       </c>
-      <c r="C52">
+      <c r="C52" t="n">
         <v>99987.484</v>
       </c>
-      <c r="D52">
+      <c r="D52" t="n">
         <v>94467.014</v>
       </c>
-      <c r="E52">
+      <c r="E52" t="n">
         <v>105.844</v>
       </c>
-      <c r="F52">
+      <c r="F52" t="n">
         <v>18.789</v>
       </c>
-      <c r="G52">
+      <c r="G52" t="n">
         <v>2.232</v>
       </c>
-      <c r="H52">
+      <c r="H52" t="n">
         <v>66.889</v>
       </c>
-      <c r="I52">
+      <c r="I52" t="n">
         <v>12.9388705634889</v>
       </c>
-      <c r="J52">
+      <c r="J52" t="n">
         <v>0.65</v>
       </c>
-      <c r="K52">
+      <c r="K52" t="n">
         <v>196709621849.5862</v>
       </c>
-      <c r="L52">
+      <c r="L52" t="n">
         <v>6.78307785917094</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
-      <c r="A53">
+    <row r="53">
+      <c r="A53" t="n">
         <v>2011</v>
       </c>
-      <c r="B53">
+      <c r="B53" t="n">
         <v>198602.738</v>
       </c>
-      <c r="C53">
+      <c r="C53" t="n">
         <v>102047.023</v>
       </c>
-      <c r="D53">
+      <c r="D53" t="n">
         <v>96555.715</v>
       </c>
-      <c r="E53">
+      <c r="E53" t="n">
         <v>105.687</v>
       </c>
-      <c r="F53">
+      <c r="F53" t="n">
         <v>18.962</v>
       </c>
-      <c r="G53">
+      <c r="G53" t="n">
         <v>1.992</v>
       </c>
-      <c r="H53">
+      <c r="H53" t="n">
         <v>67.066</v>
       </c>
-      <c r="I53">
+      <c r="I53" t="n">
         <v>11.9160927116277</v>
       </c>
-      <c r="J53">
+      <c r="J53" t="n">
         <v>0.8</v>
       </c>
-      <c r="K53">
+      <c r="K53" t="n">
         <v>230586581059.6654</v>
       </c>
-      <c r="L53">
+      <c r="L53" t="n">
         <v>6.97875575109141</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
-      <c r="A54">
+    <row r="54">
+      <c r="A54" t="n">
         <v>2012</v>
       </c>
-      <c r="B54">
+      <c r="B54" t="n">
         <v>202205.861</v>
       </c>
-      <c r="C54">
+      <c r="C54" t="n">
         <v>103831.984</v>
       </c>
-      <c r="D54">
+      <c r="D54" t="n">
         <v>98373.87699999999</v>
       </c>
-      <c r="E54">
+      <c r="E54" t="n">
         <v>105.548</v>
       </c>
-      <c r="F54">
+      <c r="F54" t="n">
         <v>19.097</v>
       </c>
-      <c r="G54">
+      <c r="G54" t="n">
         <v>1.607</v>
       </c>
-      <c r="H54">
+      <c r="H54" t="n">
         <v>67.194</v>
       </c>
-      <c r="I54">
+      <c r="I54" t="n">
         <v>9.682351860556841</v>
       </c>
-      <c r="J54">
+      <c r="J54" t="n">
         <v>3.67</v>
       </c>
-      <c r="K54">
+      <c r="K54" t="n">
         <v>250106966104.7036</v>
       </c>
-      <c r="L54">
+      <c r="L54" t="n">
         <v>6.84747710366189</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
-      <c r="A55">
+    <row r="55">
+      <c r="A55" t="n">
         <v>2013</v>
       </c>
-      <c r="B55">
+      <c r="B55" t="n">
         <v>205337.562</v>
       </c>
-      <c r="C55">
+      <c r="C55" t="n">
         <v>105378.643</v>
       </c>
-      <c r="D55">
+      <c r="D55" t="n">
         <v>99958.91899999999</v>
       </c>
-      <c r="E55">
+      <c r="E55" t="n">
         <v>105.422</v>
       </c>
-      <c r="F55">
+      <c r="F55" t="n">
         <v>19.195</v>
       </c>
-      <c r="G55">
+      <c r="G55" t="n">
         <v>1.468</v>
       </c>
-      <c r="H55">
+      <c r="H55" t="n">
         <v>67.616</v>
       </c>
-      <c r="I55">
+      <c r="I55" t="n">
         <v>7.69215611899565</v>
       </c>
-      <c r="J55">
+      <c r="J55" t="n">
         <v>2.95</v>
       </c>
-      <c r="K55">
+      <c r="K55" t="n">
         <v>258657231672.4123</v>
       </c>
-      <c r="L55">
+      <c r="L55" t="n">
         <v>6.78736022004586</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
-      <c r="A56">
+    <row r="56">
+      <c r="A56" t="n">
         <v>2014</v>
       </c>
-      <c r="B56">
+      <c r="B56" t="n">
         <v>208251.628</v>
       </c>
-      <c r="C56">
+      <c r="C56" t="n">
         <v>106815</v>
       </c>
-      <c r="D56">
+      <c r="D56" t="n">
         <v>101436.628</v>
       </c>
-      <c r="E56">
+      <c r="E56" t="n">
         <v>105.302</v>
       </c>
-      <c r="F56">
+      <c r="F56" t="n">
         <v>19.281</v>
       </c>
-      <c r="G56">
+      <c r="G56" t="n">
         <v>1.352</v>
       </c>
-      <c r="H56">
+      <c r="H56" t="n">
         <v>67.718</v>
       </c>
-      <c r="I56">
+      <c r="I56" t="n">
         <v>7.18938402847028</v>
       </c>
-      <c r="J56">
+      <c r="J56" t="n">
         <v>1.83</v>
       </c>
-      <c r="K56">
+      <c r="K56" t="n">
         <v>271390474857.6322</v>
       </c>
-      <c r="L56">
+      <c r="L56" t="n">
         <v>6.37498019073104</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
-      <c r="A57">
+    <row r="57">
+      <c r="A57" t="n">
         <v>2015</v>
       </c>
-      <c r="B57">
+      <c r="B57" t="n">
         <v>210969.298</v>
       </c>
-      <c r="C57">
+      <c r="C57" t="n">
         <v>107983.708</v>
       </c>
-      <c r="D57">
+      <c r="D57" t="n">
         <v>102985.59</v>
       </c>
-      <c r="E57">
+      <c r="E57" t="n">
         <v>104.853</v>
       </c>
-      <c r="F57">
+      <c r="F57" t="n">
         <v>19.36</v>
       </c>
-      <c r="G57">
+      <c r="G57" t="n">
         <v>1.242</v>
       </c>
-      <c r="H57">
+      <c r="H57" t="n">
         <v>68.169</v>
       </c>
-      <c r="I57">
+      <c r="I57" t="n">
         <v>2.52932817254229</v>
       </c>
-      <c r="J57">
+      <c r="J57" t="n">
         <v>3.57</v>
       </c>
-      <c r="K57">
+      <c r="K57" t="n">
         <v>299963590534.7735</v>
       </c>
-      <c r="L57">
+      <c r="L57" t="n">
         <v>4.49638885369946</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
-      <c r="A58">
+    <row r="58">
+      <c r="A58" t="n">
         <v>2016</v>
       </c>
-      <c r="B58">
+      <c r="B58" t="n">
         <v>213524.84</v>
       </c>
-      <c r="C58">
+      <c r="C58" t="n">
         <v>108894.512</v>
       </c>
-      <c r="D58">
+      <c r="D58" t="n">
         <v>104630.327</v>
       </c>
-      <c r="E58">
+      <c r="E58" t="n">
         <v>104.075</v>
       </c>
-      <c r="F58">
+      <c r="F58" t="n">
         <v>19.43</v>
       </c>
-      <c r="G58">
+      <c r="G58" t="n">
         <v>1.166</v>
       </c>
-      <c r="H58">
+      <c r="H58" t="n">
         <v>68.325</v>
       </c>
-      <c r="I58">
+      <c r="I58" t="n">
         <v>3.7651191635658</v>
       </c>
-      <c r="J58">
+      <c r="J58" t="n">
         <v>2.29</v>
       </c>
-      <c r="K58">
+      <c r="K58" t="n">
         <v>313630000130.4354</v>
       </c>
-      <c r="L58">
+      <c r="L58" t="n">
         <v>3.98829476698892</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
-      <c r="A59">
+    <row r="59">
+      <c r="A59" t="n">
         <v>2017</v>
       </c>
-      <c r="B59">
+      <c r="B59" t="n">
         <v>216379.655</v>
       </c>
-      <c r="C59">
+      <c r="C59" t="n">
         <v>110003.086</v>
       </c>
-      <c r="D59">
+      <c r="D59" t="n">
         <v>106376.569</v>
       </c>
-      <c r="E59">
+      <c r="E59" t="n">
         <v>103.409</v>
       </c>
-      <c r="F59">
+      <c r="F59" t="n">
         <v>19.523</v>
       </c>
-      <c r="G59">
+      <c r="G59" t="n">
         <v>1.488</v>
       </c>
-      <c r="H59">
+      <c r="H59" t="n">
         <v>68.816</v>
       </c>
-      <c r="I59">
+      <c r="I59" t="n">
         <v>4.08537368032608</v>
       </c>
-      <c r="J59">
+      <c r="J59" t="n">
         <v>3.187</v>
       </c>
-      <c r="K59">
+      <c r="K59" t="n">
         <v>339205534861.1001</v>
       </c>
-      <c r="L59">
+      <c r="L59" t="n">
         <v>3.80581067106332</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
-      <c r="A60">
+    <row r="60">
+      <c r="A60" t="n">
         <v>2018</v>
       </c>
-      <c r="B60">
+      <c r="B60" t="n">
         <v>219731.479</v>
       </c>
-      <c r="C60">
+      <c r="C60" t="n">
         <v>111438.323</v>
       </c>
-      <c r="D60">
+      <c r="D60" t="n">
         <v>108293.156</v>
       </c>
-      <c r="E60">
+      <c r="E60" t="n">
         <v>102.904</v>
       </c>
-      <c r="F60">
+      <c r="F60" t="n">
         <v>19.653</v>
       </c>
-      <c r="G60">
+      <c r="G60" t="n">
         <v>1.586</v>
       </c>
-      <c r="H60">
+      <c r="H60" t="n">
         <v>68.959</v>
       </c>
-      <c r="I60">
+      <c r="I60" t="n">
         <v>5.07805725868917</v>
       </c>
-      <c r="J60">
+      <c r="J60" t="n">
         <v>4.08</v>
       </c>
-      <c r="K60">
+      <c r="K60" t="n">
         <v>356128166704.921</v>
       </c>
-      <c r="L60">
+      <c r="L60" t="n">
         <v>3.75048673897451</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
-      <c r="A61">
+    <row r="61">
+      <c r="A61" t="n">
         <v>2019</v>
       </c>
-      <c r="B61">
+      <c r="B61" t="n">
         <v>223293.28</v>
       </c>
-      <c r="C61">
+      <c r="C61" t="n">
         <v>113015.042</v>
       </c>
-      <c r="D61">
+      <c r="D61" t="n">
         <v>110278.237</v>
       </c>
-      <c r="E61">
+      <c r="E61" t="n">
         <v>102.482</v>
       </c>
-      <c r="F61">
+      <c r="F61" t="n">
         <v>19.801</v>
       </c>
-      <c r="G61">
+      <c r="G61" t="n">
         <v>1.63</v>
       </c>
-      <c r="H61">
+      <c r="H61" t="n">
         <v>69.096</v>
       </c>
-      <c r="I61">
+      <c r="I61" t="n">
         <v>10.5783618004555</v>
       </c>
-      <c r="J61">
+      <c r="J61" t="n">
         <v>4.83</v>
       </c>
-      <c r="K61">
+      <c r="K61" t="n">
         <v>320909472770.6687</v>
       </c>
-      <c r="L61">
-        <v>3.65125185059589</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12">
-      <c r="A62">
+      <c r="L61" t="n">
+        <v>3.65125185059589</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
         <v>2020</v>
       </c>
-      <c r="B62">
+      <c r="B62" t="n">
         <v>227196.741</v>
       </c>
-      <c r="C62">
+      <c r="C62" t="n">
         <v>114815.641</v>
       </c>
-      <c r="D62">
+      <c r="D62" t="n">
         <v>112381.099</v>
       </c>
-      <c r="E62">
+      <c r="E62" t="n">
         <v>102.166</v>
       </c>
-      <c r="F62">
+      <c r="F62" t="n">
         <v>19.974</v>
       </c>
-      <c r="G62">
+      <c r="G62" t="n">
         <v>1.834</v>
       </c>
-      <c r="H62">
+      <c r="H62" t="n">
         <v>68.825</v>
       </c>
-      <c r="I62">
+      <c r="I62" t="n">
         <v>9.73999313898155</v>
       </c>
-      <c r="J62">
+      <c r="J62" t="n">
         <v>6.215</v>
       </c>
-      <c r="K62">
+      <c r="K62" t="n">
         <v>300425609817.9812</v>
       </c>
-      <c r="L62">
+      <c r="L62" t="n">
         <v>3.73684938494969</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
-      <c r="A63">
+    <row r="63">
+      <c r="A63" t="n">
         <v>2021</v>
       </c>
-      <c r="B63">
+      <c r="B63" t="n">
         <v>231402.117</v>
       </c>
-      <c r="C63">
+      <c r="C63" t="n">
         <v>116815.852</v>
       </c>
-      <c r="D63">
+      <c r="D63" t="n">
         <v>114586.264</v>
       </c>
-      <c r="E63">
+      <c r="E63" t="n">
         <v>101.946</v>
       </c>
-      <c r="F63">
+      <c r="F63" t="n">
         <v>20.167</v>
       </c>
-      <c r="G63">
+      <c r="G63" t="n">
         <v>1.834</v>
       </c>
-      <c r="H63">
+      <c r="H63" t="n">
         <v>68.623</v>
       </c>
-      <c r="I63">
+      <c r="I63" t="n">
         <v>9.49621056124947</v>
       </c>
-      <c r="J63">
+      <c r="J63" t="n">
         <v>6.34</v>
       </c>
-      <c r="K63">
+      <c r="K63" t="n">
         <v>348516647445.1484</v>
       </c>
-      <c r="L63">
+      <c r="L63" t="n">
         <v>3.97878815425614</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>